<commit_message>
new classifier wtihout log and samp
</commit_message>
<xml_diff>
--- a/Outputs/Results.xlsx
+++ b/Outputs/Results.xlsx
@@ -392,7 +392,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:X24"/>
+  <dimension ref="A1:X28"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
       <selection activeCell="B20" sqref="B20"/>
@@ -2973,6 +2973,430 @@
         <v>0.0198745299697441</v>
       </c>
     </row>
+    <row r="25">
+      <c r="A25" s="6" t="n">
+        <v>44329.70425930872</v>
+      </c>
+      <c r="B25" t="inlineStr">
+        <is>
+          <t>ContainsConstraints</t>
+        </is>
+      </c>
+      <c r="C25" t="inlineStr">
+        <is>
+          <t>ones</t>
+        </is>
+      </c>
+      <c r="D25" t="inlineStr">
+        <is>
+          <t>GaussianNB</t>
+        </is>
+      </c>
+      <c r="E25" t="inlineStr">
+        <is>
+          <t>RelationNum,AttributeNum,is_abstract,ObjectsNum,inherits,ObjectID,O0,O1,O2,O3,O4,O5,O6,O7,O8,O9,O10,O11,O12,O13,O14,O15,O16,O17,O18,O19,O20,O21,O22,O23,O24,O25,O26,O27,O28,O29,O30,O31,O32,O33,O34,O35,O36,O37,O38,O39,O40,O41,O42,O43,O44,O45,O46,O47,O48,O49,O50,O51,O52,O53,O54,O55,O56,O57,O58,O59,O60,O61,O62,O63,O64,O65,O66,O67,O68,O69,O70,O71,O72</t>
+        </is>
+      </c>
+      <c r="F25" t="inlineStr">
+        <is>
+          <t>under</t>
+        </is>
+      </c>
+      <c r="G25" t="n">
+        <v>0.2</v>
+      </c>
+      <c r="H25" t="n">
+        <v>10</v>
+      </c>
+      <c r="I25" t="inlineStr">
+        <is>
+          <t>True</t>
+        </is>
+      </c>
+      <c r="J25" t="inlineStr">
+        <is>
+          <t>False</t>
+        </is>
+      </c>
+      <c r="K25" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
+      <c r="L25" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
+      <c r="M25" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
+      <c r="N25" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
+      <c r="O25" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
+      <c r="P25" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
+      <c r="Q25" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
+      <c r="R25" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
+      <c r="S25" t="n">
+        <v>1</v>
+      </c>
+      <c r="T25" t="inlineStr">
+        <is>
+          <t>False</t>
+        </is>
+      </c>
+      <c r="U25" t="n">
+        <v>0.5302813543156891</v>
+      </c>
+      <c r="V25" t="n">
+        <v>0.539047619047619</v>
+      </c>
+      <c r="W25" t="n">
+        <v>0.5236067441330599</v>
+      </c>
+      <c r="X25" t="n">
+        <v>0.0141226134412093</v>
+      </c>
+    </row>
+    <row r="26">
+      <c r="A26" s="6" t="n">
+        <v>44329.70507487636</v>
+      </c>
+      <c r="B26" t="inlineStr">
+        <is>
+          <t>ContainsConstraints</t>
+        </is>
+      </c>
+      <c r="C26" t="inlineStr">
+        <is>
+          <t>ones</t>
+        </is>
+      </c>
+      <c r="D26" t="inlineStr">
+        <is>
+          <t>GaussianNB</t>
+        </is>
+      </c>
+      <c r="E26" t="inlineStr">
+        <is>
+          <t>RelationNum,AttributeNum,is_abstract,ObjectsNum,inherits,ObjectID,O0,O1,O2,O3,O4,O5,O6,O7,O8,O9,O10,O11,O12,O13,O14,O15,O16,O17,O18,O19,O20,O21,O22,O23,O24,O25,O26,O27,O28,O29,O30,O31,O32,O33,O34,O35,O36,O37,O38,O39,O40,O41,O42,O43,O44,O45,O46,O47,O48,O49,O50,O51,O52,O53,O54,O55,O56,O57,O58,O59,O60,O61,O62,O63,O64,O65,O66,O67,O68,O69,O70,O71,O72</t>
+        </is>
+      </c>
+      <c r="F26" t="inlineStr">
+        <is>
+          <t>under</t>
+        </is>
+      </c>
+      <c r="G26" t="n">
+        <v>0.2</v>
+      </c>
+      <c r="H26" t="n">
+        <v>10</v>
+      </c>
+      <c r="I26" t="inlineStr">
+        <is>
+          <t>True</t>
+        </is>
+      </c>
+      <c r="J26" t="inlineStr">
+        <is>
+          <t>False</t>
+        </is>
+      </c>
+      <c r="K26" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
+      <c r="L26" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
+      <c r="M26" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
+      <c r="N26" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
+      <c r="O26" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
+      <c r="P26" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
+      <c r="Q26" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
+      <c r="R26" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
+      <c r="S26" t="n">
+        <v>1</v>
+      </c>
+      <c r="T26" t="inlineStr">
+        <is>
+          <t>False</t>
+        </is>
+      </c>
+      <c r="U26" t="n">
+        <v>0.5317119694802098</v>
+      </c>
+      <c r="V26" t="n">
+        <v>0.5276190476190477</v>
+      </c>
+      <c r="W26" t="n">
+        <v>0.5259968102073366</v>
+      </c>
+      <c r="X26" t="n">
+        <v>0.01574221691759439</v>
+      </c>
+    </row>
+    <row r="27">
+      <c r="A27" s="6" t="n">
+        <v>44329.70704018058</v>
+      </c>
+      <c r="B27" t="inlineStr">
+        <is>
+          <t>ContainsConstraints</t>
+        </is>
+      </c>
+      <c r="C27" t="inlineStr">
+        <is>
+          <t>ones</t>
+        </is>
+      </c>
+      <c r="D27" t="inlineStr">
+        <is>
+          <t>KNeighborsClassifier</t>
+        </is>
+      </c>
+      <c r="E27" t="inlineStr">
+        <is>
+          <t>RelationNum,AttributeNum,is_abstract,ObjectsNum,inherits,ObjectID,O0,O1,O2,O3,O4,O5,O6,O7,O8,O9,O10,O11,O12,O13,O14,O15,O16,O17,O18,O19,O20,O21,O22,O23,O24,O25,O26,O27,O28,O29,O30,O31,O32,O33,O34,O35,O36,O37,O38,O39,O40,O41,O42,O43,O44,O45,O46,O47,O48,O49,O50,O51,O52,O53,O54,O55,O56,O57,O58,O59,O60,O61,O62,O63,O64,O65,O66,O67,O68,O69,O70,O71,O72</t>
+        </is>
+      </c>
+      <c r="F27" t="inlineStr">
+        <is>
+          <t>under</t>
+        </is>
+      </c>
+      <c r="G27" t="n">
+        <v>0.2</v>
+      </c>
+      <c r="H27" t="n">
+        <v>10</v>
+      </c>
+      <c r="I27" t="inlineStr">
+        <is>
+          <t>True</t>
+        </is>
+      </c>
+      <c r="J27" t="inlineStr">
+        <is>
+          <t>False</t>
+        </is>
+      </c>
+      <c r="K27" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
+      <c r="L27" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
+      <c r="M27" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
+      <c r="N27" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
+      <c r="O27" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
+      <c r="P27" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
+      <c r="Q27" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
+      <c r="R27" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
+      <c r="S27" t="n">
+        <v>1</v>
+      </c>
+      <c r="T27" t="inlineStr">
+        <is>
+          <t>False</t>
+        </is>
+      </c>
+      <c r="U27" t="n">
+        <v>0.7544110634239389</v>
+      </c>
+      <c r="V27" t="n">
+        <v>0.5847619047619048</v>
+      </c>
+      <c r="W27" t="n">
+        <v>0.5965573023467761</v>
+      </c>
+      <c r="X27" t="n">
+        <v>0.02429341554201177</v>
+      </c>
+    </row>
+    <row r="28">
+      <c r="A28" s="6" t="n">
+        <v>44329.71761315443</v>
+      </c>
+      <c r="B28" t="inlineStr">
+        <is>
+          <t>ContainsConstraints</t>
+        </is>
+      </c>
+      <c r="C28" t="inlineStr">
+        <is>
+          <t>ones</t>
+        </is>
+      </c>
+      <c r="D28" t="inlineStr">
+        <is>
+          <t>RandomForestClassifier</t>
+        </is>
+      </c>
+      <c r="E28" t="inlineStr">
+        <is>
+          <t>RelationNum,AttributeNum,is_abstract,ObjectsNum,inherits,ObjectID,O0,O1,O2,O3,O4,O5,O6,O7,O8,O9,O10,O11,O12,O13,O14,O15,O16,O17,O18,O19,O20,O21,O22,O23,O24,O25,O26,O27,O28,O29,O30,O31,O32,O33,O34,O35,O36,O37,O38,O39,O40,O41,O42,O43,O44,O45,O46,O47,O48,O49,O50,O51,O52,O53,O54,O55,O56,O57,O58,O59,O60,O61,O62,O63,O64,O65,O66,O67,O68,O69,O70,O71,O72</t>
+        </is>
+      </c>
+      <c r="F28" t="inlineStr">
+        <is>
+          <t>under</t>
+        </is>
+      </c>
+      <c r="G28" t="n">
+        <v>0.2</v>
+      </c>
+      <c r="H28" t="n">
+        <v>10</v>
+      </c>
+      <c r="I28" t="inlineStr">
+        <is>
+          <t>True</t>
+        </is>
+      </c>
+      <c r="J28" t="inlineStr">
+        <is>
+          <t>False</t>
+        </is>
+      </c>
+      <c r="K28" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
+      <c r="L28" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
+      <c r="M28" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
+      <c r="N28" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
+      <c r="O28" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
+      <c r="P28" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
+      <c r="Q28" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
+      <c r="R28" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
+      <c r="S28" t="n">
+        <v>1</v>
+      </c>
+      <c r="T28" t="inlineStr">
+        <is>
+          <t>False</t>
+        </is>
+      </c>
+      <c r="U28" t="n">
+        <v>0.9461134954697187</v>
+      </c>
+      <c r="V28" t="n">
+        <v>0.6895238095238095</v>
+      </c>
+      <c r="W28" t="n">
+        <v>0.6852813852813854</v>
+      </c>
+      <c r="X28" t="n">
+        <v>0.01520280763386198</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
   <pageSetup orientation="portrait"/>

</xml_diff>